<commit_message>
Verified matrix order and orientation in each equation using Matlab SVD (see /tests/PCAtesting.m) and updated figures and equations to reflect this. Also changed the figure shape to suit the majority of figures.
</commit_message>
<xml_diff>
--- a/docs/Notation.xlsx
+++ b/docs/Notation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Algo\Jupyter\PCA\PCAMath.git\trunk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848B542F-6217-4FDB-B597-F68A4074EB71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E370931E-AD5D-4FE9-B7A5-2F62053EE3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>p - number of variables - change to m?</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>X, D, Data, Spectra</t>
+  </si>
+  <si>
+    <t>ix</t>
+  </si>
+  <si>
+    <t>non code index e.g. PCA number - starts at 1. This is the most expected index for use outside of zero indexed coding. Used in script to choose PC index etc</t>
+  </si>
+  <si>
+    <t>Zero-indexed coding - this will delineate between code index and other types of index. Always convert i index input into ix index at start of any functions using it.</t>
   </si>
 </sst>
 </file>
@@ -813,10 +822,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF07D412-D2F6-4D4C-A226-4E1951F3499A}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,6 +919,22 @@
         <v>61</v>
       </c>
     </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Added comments to local_nipals.py
Regenerated figures after fixing my jupyter environment.
Added comments into the readme to avoid .env issues.
Added comments to spreadsheet regarding variable names.
</commit_message>
<xml_diff>
--- a/docs/Notation.xlsx
+++ b/docs/Notation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Algo\Jupyter\PCA\PCAMath.git\trunk\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\Papers\2019_Rene_Beattie\PCAMath\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E370931E-AD5D-4FE9-B7A5-2F62053EE3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92A3C42-C059-49E3-8C6C-3E035E4A1D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
+    <workbookView xWindow="-27435" yWindow="-1440" windowWidth="26925" windowHeight="14640" activeTab="1" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Math" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>p - number of variables - change to m?</t>
   </si>
@@ -239,14 +238,76 @@
   </si>
   <si>
     <t>Zero-indexed coding - this will delineate between code index and other types of index. Always convert i index input into ix index at start of any functions using it.</t>
+  </si>
+  <si>
+    <t>component_weight</t>
+  </si>
+  <si>
+    <t>Python variable</t>
+  </si>
+  <si>
+    <t>Math Notation</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>component_index</t>
+  </si>
+  <si>
+    <t>spectral_loading</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>positive_sum</t>
+  </si>
+  <si>
+    <t>negative_sum</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>spectral data</t>
+  </si>
+  <si>
+    <t>Francis' suggestions</t>
+  </si>
+  <si>
+    <t>Use what's present in most of the existing manuscript &amp; figures.</t>
+  </si>
+  <si>
+    <t>spectral component loadings</t>
+  </si>
+  <si>
+    <t>component concentration scores</t>
+  </si>
+  <si>
+    <t>positive contributions</t>
+  </si>
+  <si>
+    <t>negative contributions</t>
+  </si>
+  <si>
+    <t>central contribution offset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -274,10 +335,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,120 +890,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF07D412-D2F6-4D4C-A226-4E1951F3499A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="94.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I3:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated notation used in equations and figures to that described in notation.xlsx
</commit_message>
<xml_diff>
--- a/docs/Notation.xlsx
+++ b/docs/Notation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\Papers\2019_Rene_Beattie\PCAMath\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Algo\Jupyter\PCA\PCAMath.git\trunk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92A3C42-C059-49E3-8C6C-3E035E4A1D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3625AA5B-42C3-4BE5-A6E9-65010020AFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27435" yWindow="-1440" windowWidth="26925" windowHeight="14640" activeTab="1" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
+    <workbookView xWindow="44430" yWindow="-9915" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Math" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="106">
   <si>
     <t>p - number of variables - change to m?</t>
   </si>
@@ -292,13 +292,70 @@
   </si>
   <si>
     <t>central contribution offset</t>
+  </si>
+  <si>
+    <t>Number of PCs/dimensionality</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>f for number of factors</t>
+  </si>
+  <si>
+    <t>^\top</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>multiplication</t>
+  </si>
+  <si>
+    <t>\times</t>
+  </si>
+  <si>
+    <t>conventional mathemetical notation</t>
+  </si>
+  <si>
+    <t>Conditional statement</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Iverson Brackets</t>
+  </si>
+  <si>
+    <t>elements conditional on positive score</t>
+  </si>
+  <si>
+    <t>_{p+}</t>
+  </si>
+  <si>
+    <t>loading or score for pth PC from positive score spectra</t>
+  </si>
+  <si>
+    <t>elements conditional on negative score</t>
+  </si>
+  <si>
+    <t>_{p-}</t>
+  </si>
+  <si>
+    <t>loading or score for pth PC from negative score spectra</t>
+  </si>
+  <si>
+    <t>covariance matrix</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +367,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -347,6 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405F8C9B-81B4-4F77-9B95-F29E55E7334B}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,7 +739,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
@@ -688,7 +753,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -702,7 +767,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
@@ -716,91 +781,91 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>19</v>
+      <c r="A9" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
@@ -814,7 +879,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
@@ -828,7 +893,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
@@ -842,7 +907,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
@@ -856,21 +921,21 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
@@ -881,6 +946,79 @@
       </c>
       <c r="D15" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -893,7 +1031,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
verified that the rearranged equations could be replicated in code, updated variable names in code to reflect Notation.xlsx. Updated some sections of workbook.
</commit_message>
<xml_diff>
--- a/docs/Notation.xlsx
+++ b/docs/Notation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Algo\Jupyter\PCA\PCAMath.git\trunk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3625AA5B-42C3-4BE5-A6E9-65010020AFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9780D00E-E115-4C83-8076-03596C84174D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44430" yWindow="-9915" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E3967C3F-9CF9-4968-BB60-077DDD953DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Math" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>p - number of variables - change to m?</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>orthogonal_sum</t>
+  </si>
+  <si>
+    <t>component_array_index</t>
   </si>
 </sst>
 </file>
@@ -408,10 +414,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405F8C9B-81B4-4F77-9B95-F29E55E7334B}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -739,7 +745,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
@@ -753,7 +759,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -767,7 +773,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
@@ -781,7 +787,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
@@ -795,7 +801,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
@@ -809,7 +815,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -823,7 +829,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
@@ -837,7 +843,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
@@ -851,7 +857,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
@@ -865,7 +871,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
@@ -879,7 +885,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
@@ -893,7 +899,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
@@ -907,7 +913,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
@@ -921,7 +927,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
@@ -935,7 +941,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
@@ -949,7 +955,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B16" t="s">
@@ -963,7 +969,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>95</v>
       </c>
@@ -975,7 +981,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -989,7 +995,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>98</v>
       </c>
@@ -1001,7 +1007,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>101</v>
       </c>
@@ -1013,7 +1019,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>104</v>
       </c>
@@ -1030,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF07D412-D2F6-4D4C-A226-4E1951F3499A}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1107,7 @@
       <c r="H3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1124,7 +1130,7 @@
       <c r="H4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1145,7 +1151,7 @@
       <c r="H5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1195,6 +1201,9 @@
       <c r="C8" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>86</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>